<commit_message>
Add test add company
</commit_message>
<xml_diff>
--- a/dataTest/Data_testLogin.xlsx
+++ b/dataTest/Data_testLogin.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Readme\New folder\Test_Login_WebCompanyManage\dataTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tester\TestPOM\dataTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81CB15-2762-4E9C-834E-5E40FA65B132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB710394-8F8F-4312-A34A-42465CAB27B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="2208" windowWidth="17280" windowHeight="8880" xr2:uid="{0D890ACC-771F-45E4-B40E-A07B34AC1F8C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D890ACC-771F-45E4-B40E-A07B34AC1F8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,34 +45,34 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>tester@gmail.com</t>
+  </si>
+  <si>
+    <t>password must contain at least 1 letter and 1 number</t>
+  </si>
+  <si>
+    <t>Test1234</t>
+  </si>
+  <si>
     <t>Incorrect email or password!</t>
   </si>
   <si>
-    <t>tester@gmail.com</t>
+    <t>ab123</t>
+  </si>
+  <si>
+    <t>password must be at least 6 characters</t>
+  </si>
+  <si>
+    <t>"password" is not allowed to be empty</t>
   </si>
   <si>
     <t>"email" is not allowed to be empty</t>
-  </si>
-  <si>
-    <t>"password" is not allowed to be empty</t>
-  </si>
-  <si>
-    <t>password must contain at least 1 letter and 1 number</t>
-  </si>
-  <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>Test1234</t>
-  </si>
-  <si>
-    <t>admin@gmail.com</t>
-  </si>
-  <si>
-    <t>ab123</t>
-  </si>
-  <si>
-    <t>password must be at least 6 characters</t>
   </si>
 </sst>
 </file>
@@ -123,7 +123,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -443,7 +443,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,36 +476,37 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
+      <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
+      <c r="B3" t="s">
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -514,83 +515,83 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
+      <c r="B6" t="s">
+        <v>6</v>
       </c>
       <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
         <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
+      <c r="B7" t="s">
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
+      <c r="B9" t="s">
+        <v>8</v>
       </c>
       <c r="C9">
         <v>123456</v>
@@ -599,15 +600,11 @@
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{8980C724-7086-4FD6-B3A2-60E685837DBC}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{1E04CCF0-0620-4E3C-A265-AEC9D085B1D4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>